<commit_message>
a lot of stuff sry
</commit_message>
<xml_diff>
--- a/Dokumentation/GroupAssignment.xlsx
+++ b/Dokumentation/GroupAssignment.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a3af9c331d4dfead/Documents/Studium Informatik B.Sc/SS2024/Software Praktikum/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a3af9c331d4dfead/Documents/Studium Informatik B.Sc/SS2024/Software Praktikum/Project/Dokumentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="275" documentId="8_{3BCD1BE3-B716-47D2-9CFE-8E76072B354A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8BFF980-2CAE-4F84-8D2C-003F601EEFA6}"/>
+  <xr:revisionPtr revIDLastSave="304" documentId="8_{3BCD1BE3-B716-47D2-9CFE-8E76072B354A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A03E9C95-B14B-4BC5-8297-FA6BD9AC32E6}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6BE980AD-1C3C-443A-8FC3-D26A02B01641}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>Ablauf</t>
   </si>
@@ -118,6 +118,15 @@
   </si>
   <si>
     <t>Diagramm</t>
+  </si>
+  <si>
+    <t>Konzept für Umsetzung</t>
+  </si>
+  <si>
+    <t>Umsetzung für konzept</t>
+  </si>
+  <si>
+    <t>Testen</t>
   </si>
 </sst>
 </file>
@@ -238,7 +247,112 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="27">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -334,10 +448,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -663,7 +773,7 @@
   <dimension ref="A1:CX29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1967,89 +2077,339 @@
       </c>
     </row>
     <row r="16" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10"/>
-      <c r="S16" s="10"/>
-      <c r="T16" s="10"/>
-      <c r="U16" s="10"/>
-      <c r="V16" s="10"/>
-      <c r="W16" s="10"/>
-      <c r="X16" s="10"/>
-      <c r="Y16" s="10"/>
-      <c r="Z16" s="10"/>
-      <c r="AA16" s="10"/>
-      <c r="AB16" s="10"/>
-      <c r="AC16" s="10"/>
-      <c r="AD16" s="10"/>
-      <c r="AE16" s="10"/>
-      <c r="AF16" s="10"/>
-      <c r="AG16" s="10"/>
-    </row>
-    <row r="17" spans="2:33" x14ac:dyDescent="0.35">
-      <c r="C17" s="11"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="12"/>
-      <c r="Q17" s="12"/>
-      <c r="R17" s="12"/>
-      <c r="S17" s="12"/>
-      <c r="T17" s="12"/>
-      <c r="U17" s="12"/>
-      <c r="V17" s="12"/>
-      <c r="W17" s="12"/>
-      <c r="X17" s="12"/>
-      <c r="Y17" s="12"/>
-      <c r="Z17" s="12"/>
-      <c r="AA17" s="12"/>
-      <c r="AB17" s="12"/>
-      <c r="AC17" s="12"/>
-      <c r="AD17" s="12"/>
-      <c r="AE17" s="12"/>
-      <c r="AF17" s="12"/>
-      <c r="AG17" s="12"/>
-    </row>
-    <row r="18" spans="2:33" x14ac:dyDescent="0.35">
-      <c r="B18" s="1"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:33" x14ac:dyDescent="0.35">
-      <c r="B19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:33" x14ac:dyDescent="0.35">
-      <c r="B20" s="1"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:33" x14ac:dyDescent="0.35">
-      <c r="B21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:33" x14ac:dyDescent="0.35">
-      <c r="B22" s="1"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:33" x14ac:dyDescent="0.35">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="5" t="str">
+        <f t="shared" ref="E16:AG16" si="9">TEXT(E17,"TTT")</f>
+        <v>Do</v>
+      </c>
+      <c r="F16" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>Fr</v>
+      </c>
+      <c r="G16" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>Sa</v>
+      </c>
+      <c r="H16" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>So</v>
+      </c>
+      <c r="I16" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>Mo</v>
+      </c>
+      <c r="J16" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>Di</v>
+      </c>
+      <c r="K16" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>Mi</v>
+      </c>
+      <c r="L16" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>Do</v>
+      </c>
+      <c r="M16" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>Fr</v>
+      </c>
+      <c r="N16" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>Sa</v>
+      </c>
+      <c r="O16" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>So</v>
+      </c>
+      <c r="P16" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>Mo</v>
+      </c>
+      <c r="Q16" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>Di</v>
+      </c>
+      <c r="R16" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>Mi</v>
+      </c>
+      <c r="S16" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>Do</v>
+      </c>
+      <c r="T16" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>Fr</v>
+      </c>
+      <c r="U16" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>Sa</v>
+      </c>
+      <c r="V16" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>So</v>
+      </c>
+      <c r="W16" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>Mo</v>
+      </c>
+      <c r="X16" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>Di</v>
+      </c>
+      <c r="Y16" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>Mi</v>
+      </c>
+      <c r="Z16" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>Do</v>
+      </c>
+      <c r="AA16" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>Fr</v>
+      </c>
+      <c r="AB16" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>Sa</v>
+      </c>
+      <c r="AC16" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>So</v>
+      </c>
+      <c r="AD16" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>Mo</v>
+      </c>
+      <c r="AE16" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>Di</v>
+      </c>
+      <c r="AF16" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>Mi</v>
+      </c>
+      <c r="AG16" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>Do</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="7">
+        <f>B6</f>
+        <v>45428</v>
+      </c>
+      <c r="F17" s="7">
+        <f>E17+1</f>
+        <v>45429</v>
+      </c>
+      <c r="G17" s="7">
+        <f t="shared" ref="G17" si="10">F17+1</f>
+        <v>45430</v>
+      </c>
+      <c r="H17" s="7">
+        <f t="shared" ref="H17" si="11">G17+1</f>
+        <v>45431</v>
+      </c>
+      <c r="I17" s="7">
+        <f t="shared" ref="I17" si="12">H17+1</f>
+        <v>45432</v>
+      </c>
+      <c r="J17" s="7">
+        <f t="shared" ref="J17" si="13">I17+1</f>
+        <v>45433</v>
+      </c>
+      <c r="K17" s="7">
+        <f t="shared" ref="K17" si="14">J17+1</f>
+        <v>45434</v>
+      </c>
+      <c r="L17" s="7">
+        <f t="shared" ref="L17" si="15">K17+1</f>
+        <v>45435</v>
+      </c>
+      <c r="M17" s="7">
+        <f t="shared" ref="M17" si="16">L17+1</f>
+        <v>45436</v>
+      </c>
+      <c r="N17" s="7">
+        <f t="shared" ref="N17" si="17">M17+1</f>
+        <v>45437</v>
+      </c>
+      <c r="O17" s="7">
+        <f t="shared" ref="O17" si="18">N17+1</f>
+        <v>45438</v>
+      </c>
+      <c r="P17" s="7">
+        <f t="shared" ref="P17" si="19">O17+1</f>
+        <v>45439</v>
+      </c>
+      <c r="Q17" s="7">
+        <f t="shared" ref="Q17" si="20">P17+1</f>
+        <v>45440</v>
+      </c>
+      <c r="R17" s="7">
+        <f t="shared" ref="R17" si="21">Q17+1</f>
+        <v>45441</v>
+      </c>
+      <c r="S17" s="7">
+        <f t="shared" ref="S17" si="22">R17+1</f>
+        <v>45442</v>
+      </c>
+      <c r="T17" s="7">
+        <f t="shared" ref="T17" si="23">S17+1</f>
+        <v>45443</v>
+      </c>
+      <c r="U17" s="7">
+        <f t="shared" ref="U17" si="24">T17+1</f>
+        <v>45444</v>
+      </c>
+      <c r="V17" s="7">
+        <f t="shared" ref="V17" si="25">U17+1</f>
+        <v>45445</v>
+      </c>
+      <c r="W17" s="7">
+        <f t="shared" ref="W17" si="26">V17+1</f>
+        <v>45446</v>
+      </c>
+      <c r="X17" s="7">
+        <f t="shared" ref="X17" si="27">W17+1</f>
+        <v>45447</v>
+      </c>
+      <c r="Y17" s="7">
+        <f t="shared" ref="Y17" si="28">X17+1</f>
+        <v>45448</v>
+      </c>
+      <c r="Z17" s="7">
+        <f t="shared" ref="Z17" si="29">Y17+1</f>
+        <v>45449</v>
+      </c>
+      <c r="AA17" s="7">
+        <f t="shared" ref="AA17" si="30">Z17+1</f>
+        <v>45450</v>
+      </c>
+      <c r="AB17" s="7">
+        <f t="shared" ref="AB17" si="31">AA17+1</f>
+        <v>45451</v>
+      </c>
+      <c r="AC17" s="7">
+        <f t="shared" ref="AC17" si="32">AB17+1</f>
+        <v>45452</v>
+      </c>
+      <c r="AD17" s="7">
+        <f t="shared" ref="AD17" si="33">AC17+1</f>
+        <v>45453</v>
+      </c>
+      <c r="AE17" s="7">
+        <f t="shared" ref="AE17" si="34">AD17+1</f>
+        <v>45454</v>
+      </c>
+      <c r="AF17" s="7">
+        <f t="shared" ref="AF17" si="35">AE17+1</f>
+        <v>45455</v>
+      </c>
+      <c r="AG17" s="7">
+        <f t="shared" ref="AG17" si="36">AF17+1</f>
+        <v>45456</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1">
+        <f>B6</f>
+        <v>45428</v>
+      </c>
+      <c r="C18" s="3">
+        <f>4*7</f>
+        <v>28</v>
+      </c>
+      <c r="D18" s="1">
+        <f>B18+C18</f>
+        <v>45456</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="1">
+        <f>B18</f>
+        <v>45428</v>
+      </c>
+      <c r="C19" s="3">
+        <v>7</v>
+      </c>
+      <c r="D19" s="1">
+        <f>B19+C19</f>
+        <v>45435</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="1">
+        <f>D19</f>
+        <v>45435</v>
+      </c>
+      <c r="C20" s="3">
+        <v>7</v>
+      </c>
+      <c r="D20" s="1">
+        <f>B20+C20</f>
+        <v>45442</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="1">
+        <f t="shared" ref="B21:B22" si="37">D20</f>
+        <v>45442</v>
+      </c>
+      <c r="C21" s="3">
+        <v>7</v>
+      </c>
+      <c r="D21" s="1">
+        <f>B21+C21</f>
+        <v>45449</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="1">
+        <f t="shared" si="37"/>
+        <v>45449</v>
+      </c>
+      <c r="C22" s="3">
+        <v>7</v>
+      </c>
+      <c r="D22" s="1">
+        <f>B22+C22</f>
+        <v>45456</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.35">
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
@@ -2080,7 +2440,7 @@
       <c r="AF23" s="10"/>
       <c r="AG23" s="10"/>
     </row>
-    <row r="24" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.35">
       <c r="C24" s="11"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
@@ -2112,23 +2472,23 @@
       <c r="AF24" s="12"/>
       <c r="AG24" s="12"/>
     </row>
-    <row r="25" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B29" s="1"/>
       <c r="D29" s="1"/>
     </row>
@@ -2138,47 +2498,47 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="E11:AG15">
-    <cfRule type="expression" dxfId="11" priority="22">
+    <cfRule type="expression" dxfId="26" priority="25">
       <formula>AND(E$10 &gt;=$B11, E$10 &lt;= $D11, TODAY() = E$10)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="23">
+    <cfRule type="expression" dxfId="25" priority="26">
       <formula>AND(E$10 &gt;= $B11,E$10 &lt;= $D11, TODAY() &gt; E$10)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="24">
+    <cfRule type="expression" dxfId="24" priority="27">
       <formula>AND(E$10 &gt;= $B11,E$10 &lt;= $D11)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E18:AG22">
-    <cfRule type="expression" dxfId="8" priority="4">
-      <formula>AND(E$10 &gt;=$B18, E$10 &lt;= $D18, TODAY() = E$10)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="7" priority="5">
-      <formula>AND(E$10 &gt;= $B18,E$10 &lt;= $D18, TODAY() &gt; E$10)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="6">
-      <formula>AND(E$10 &gt;= $B18,E$10 &lt;= $D18)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E25:AG29">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="23" priority="4">
       <formula>AND(E$10 &gt;=$B25, E$10 &lt;= $D25, TODAY() = E$10)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="22" priority="5">
       <formula>AND(E$10 &gt;= $B25,E$10 &lt;= $D25, TODAY() &gt; E$10)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="21" priority="6">
       <formula>AND(E$10 &gt;= $B25,E$10 &lt;= $D25)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:CW8">
-    <cfRule type="expression" dxfId="2" priority="29">
+    <cfRule type="expression" dxfId="20" priority="32">
       <formula>AND(E$3 &gt;= $B4,E$3 &lt;= $D4, TODAY() = E$3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="30">
+    <cfRule type="expression" dxfId="19" priority="33">
       <formula>AND(E$3 &gt;= $B4,E$3 &lt;= $D4, TODAY() &gt; E$3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="31">
+    <cfRule type="expression" dxfId="18" priority="34">
       <formula>AND(E$3 &gt;= $B4,E$3 &lt;= $D4)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18:AG22">
+    <cfRule type="expression" dxfId="17" priority="1">
+      <formula>AND(E$17 &gt;=$B18, E$17 &lt;= $D18, TODAY() = E$17)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="2">
+      <formula>AND(E$17 &gt;= $B18,E$17 &lt;= $D18, TODAY() &gt; E$17)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="3">
+      <formula>AND(E$17 &gt;= $B18,E$17 &lt;= $D18)</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
a whole lotta small changes for example: implementation of remove in GroupManager, disjunction of inputPeople and calc... sry
</commit_message>
<xml_diff>
--- a/Dokumentation/GroupAssignment.xlsx
+++ b/Dokumentation/GroupAssignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a3af9c331d4dfead/Documents/Studium Informatik B.Sc/SS2024/Software Praktikum/Project/Dokumentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="304" documentId="8_{3BCD1BE3-B716-47D2-9CFE-8E76072B354A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A03E9C95-B14B-4BC5-8297-FA6BD9AC32E6}"/>
+  <xr:revisionPtr revIDLastSave="305" documentId="8_{3BCD1BE3-B716-47D2-9CFE-8E76072B354A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2400DB2E-DB4F-4B5B-9B30-B1F06EB42008}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6BE980AD-1C3C-443A-8FC3-D26A02B01641}"/>
   </bookViews>
@@ -247,112 +247,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -448,6 +343,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -773,7 +672,7 @@
   <dimension ref="A1:CX29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2330,7 +2229,7 @@
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B18" s="1">
         <f>B6</f>
@@ -2498,47 +2397,47 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="E11:AG15">
-    <cfRule type="expression" dxfId="26" priority="25">
+    <cfRule type="expression" dxfId="11" priority="25">
       <formula>AND(E$10 &gt;=$B11, E$10 &lt;= $D11, TODAY() = E$10)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="26">
+    <cfRule type="expression" dxfId="10" priority="26">
       <formula>AND(E$10 &gt;= $B11,E$10 &lt;= $D11, TODAY() &gt; E$10)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="27">
+    <cfRule type="expression" dxfId="9" priority="27">
       <formula>AND(E$10 &gt;= $B11,E$10 &lt;= $D11)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E18:AG22">
+    <cfRule type="expression" dxfId="8" priority="1">
+      <formula>AND(E$17 &gt;=$B18, E$17 &lt;= $D18, TODAY() = E$17)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="2">
+      <formula>AND(E$17 &gt;= $B18,E$17 &lt;= $D18, TODAY() &gt; E$17)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="3">
+      <formula>AND(E$17 &gt;= $B18,E$17 &lt;= $D18)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="E25:AG29">
-    <cfRule type="expression" dxfId="23" priority="4">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>AND(E$10 &gt;=$B25, E$10 &lt;= $D25, TODAY() = E$10)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>AND(E$10 &gt;= $B25,E$10 &lt;= $D25, TODAY() &gt; E$10)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="6">
+    <cfRule type="expression" dxfId="3" priority="6">
       <formula>AND(E$10 &gt;= $B25,E$10 &lt;= $D25)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:CW8">
-    <cfRule type="expression" dxfId="20" priority="32">
+    <cfRule type="expression" dxfId="2" priority="32">
       <formula>AND(E$3 &gt;= $B4,E$3 &lt;= $D4, TODAY() = E$3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="33">
+    <cfRule type="expression" dxfId="1" priority="33">
       <formula>AND(E$3 &gt;= $B4,E$3 &lt;= $D4, TODAY() &gt; E$3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="34">
+    <cfRule type="expression" dxfId="0" priority="34">
       <formula>AND(E$3 &gt;= $B4,E$3 &lt;= $D4)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E18:AG22">
-    <cfRule type="expression" dxfId="17" priority="1">
-      <formula>AND(E$17 &gt;=$B18, E$17 &lt;= $D18, TODAY() = E$17)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="2">
-      <formula>AND(E$17 &gt;= $B18,E$17 &lt;= $D18, TODAY() &gt; E$17)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="15" priority="3">
-      <formula>AND(E$17 &gt;= $B18,E$17 &lt;= $D18)</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>